<commit_message>
clustering on candidates graph
</commit_message>
<xml_diff>
--- a/data/arxiv_input_probable_errata.xlsx
+++ b/data/arxiv_input_probable_errata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\PHDResearch\Dev\r\name-matching-graph-gen\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\PHDResearch\Dev\r\name-matching-data-preparation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4326,11 +4326,10 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H1015" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:H1015">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="al.kavalov"/>
-        <filter val="al.r.kavalov"/>
-      </filters>
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <sortState ref="A2:I1012">
@@ -4666,7 +4665,7 @@
   <dimension ref="A1:N1015"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1019" sqref="H1019"/>
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4708,7 +4707,7 @@
       </c>
       <c r="I1"/>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -4735,7 +4734,7 @@
       </c>
       <c r="I2"/>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -5107,7 +5106,7 @@
       <c r="H18" s="3"/>
       <c r="I18"/>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -5134,7 +5133,7 @@
       </c>
       <c r="I19"/>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -5529,7 +5528,7 @@
       <c r="H36" s="3"/>
       <c r="I36"/>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2</v>
       </c>
@@ -5554,7 +5553,7 @@
       <c r="H37" s="3"/>
       <c r="I37"/>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2</v>
       </c>
@@ -5579,7 +5578,7 @@
       <c r="H38" s="3"/>
       <c r="I38"/>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2</v>
       </c>
@@ -5604,7 +5603,7 @@
       <c r="H39" s="3"/>
       <c r="I39"/>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2</v>
       </c>
@@ -5629,7 +5628,7 @@
       <c r="H40" s="3"/>
       <c r="I40"/>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2</v>
       </c>
@@ -5654,7 +5653,7 @@
       <c r="H41" s="3"/>
       <c r="I41"/>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2</v>
       </c>
@@ -5771,7 +5770,7 @@
       <c r="H46" s="3"/>
       <c r="I46"/>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>2</v>
       </c>
@@ -5796,7 +5795,7 @@
       <c r="H47" s="3"/>
       <c r="I47"/>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>2</v>
       </c>
@@ -5821,7 +5820,7 @@
       <c r="H48" s="3"/>
       <c r="I48"/>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>2</v>
       </c>
@@ -5846,7 +5845,7 @@
       <c r="H49" s="3"/>
       <c r="I49"/>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>2</v>
       </c>
@@ -5871,7 +5870,7 @@
       <c r="H50" s="3"/>
       <c r="I50"/>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>2</v>
       </c>
@@ -6201,7 +6200,7 @@
       <c r="H64" s="3"/>
       <c r="I64"/>
     </row>
-    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>2</v>
       </c>
@@ -6226,7 +6225,7 @@
       <c r="H65" s="3"/>
       <c r="I65"/>
     </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>2</v>
       </c>
@@ -6251,7 +6250,7 @@
       <c r="H66" s="3"/>
       <c r="I66"/>
     </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>2</v>
       </c>
@@ -6437,7 +6436,7 @@
       <c r="H74" s="3"/>
       <c r="I74"/>
     </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>2</v>
       </c>
@@ -6462,7 +6461,7 @@
       <c r="H75" s="3"/>
       <c r="I75"/>
     </row>
-    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>2</v>
       </c>
@@ -6487,7 +6486,7 @@
       <c r="H76" s="3"/>
       <c r="I76"/>
     </row>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>2</v>
       </c>
@@ -6604,7 +6603,7 @@
       <c r="H81" s="3"/>
       <c r="I81"/>
     </row>
-    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>2</v>
       </c>
@@ -6629,7 +6628,7 @@
       <c r="H82" s="3"/>
       <c r="I82"/>
     </row>
-    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>2</v>
       </c>
@@ -6654,7 +6653,7 @@
       <c r="H83" s="3"/>
       <c r="I83"/>
     </row>
-    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>2</v>
       </c>
@@ -6679,7 +6678,7 @@
       <c r="H84" s="3"/>
       <c r="I84"/>
     </row>
-    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>2</v>
       </c>
@@ -6865,7 +6864,7 @@
       <c r="H92" s="3"/>
       <c r="I92"/>
     </row>
-    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>2</v>
       </c>
@@ -6890,7 +6889,7 @@
       <c r="H93" s="3"/>
       <c r="I93"/>
     </row>
-    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>2</v>
       </c>
@@ -6915,7 +6914,7 @@
       <c r="H94" s="3"/>
       <c r="I94"/>
     </row>
-    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>2</v>
       </c>
@@ -6940,7 +6939,7 @@
       <c r="H95" s="3"/>
       <c r="I95"/>
     </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>2</v>
       </c>
@@ -7015,7 +7014,7 @@
       </c>
       <c r="I98"/>
     </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>2</v>
       </c>
@@ -7040,7 +7039,7 @@
       <c r="H99" s="3"/>
       <c r="I99"/>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>2</v>
       </c>
@@ -7249,7 +7248,7 @@
       <c r="H108" s="3"/>
       <c r="I108"/>
     </row>
-    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>2</v>
       </c>
@@ -7274,7 +7273,7 @@
       <c r="H109" s="3"/>
       <c r="I109"/>
     </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>2</v>
       </c>
@@ -7299,7 +7298,7 @@
       <c r="H110" s="3"/>
       <c r="I110"/>
     </row>
-    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>2</v>
       </c>
@@ -7715,7 +7714,7 @@
       <c r="H128" s="3"/>
       <c r="I128"/>
     </row>
-    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>2</v>
       </c>
@@ -7740,7 +7739,7 @@
       <c r="H129" s="3"/>
       <c r="I129"/>
     </row>
-    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>2</v>
       </c>
@@ -7765,7 +7764,7 @@
       <c r="H130" s="3"/>
       <c r="I130"/>
     </row>
-    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>2</v>
       </c>
@@ -7790,7 +7789,7 @@
       <c r="H131" s="3"/>
       <c r="I131"/>
     </row>
-    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>2</v>
       </c>
@@ -7815,7 +7814,7 @@
       <c r="H132" s="3"/>
       <c r="I132"/>
     </row>
-    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>2</v>
       </c>
@@ -7842,7 +7841,7 @@
       </c>
       <c r="I133"/>
     </row>
-    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>2</v>
       </c>
@@ -8237,7 +8236,7 @@
       <c r="H150" s="3"/>
       <c r="I150"/>
     </row>
-    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>2</v>
       </c>
@@ -8262,7 +8261,7 @@
       <c r="H151" s="3"/>
       <c r="I151"/>
     </row>
-    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>2</v>
       </c>
@@ -8337,7 +8336,7 @@
       </c>
       <c r="I154"/>
     </row>
-    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>2</v>
       </c>
@@ -8362,7 +8361,7 @@
       <c r="H155" s="3"/>
       <c r="I155"/>
     </row>
-    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>2</v>
       </c>
@@ -8387,7 +8386,7 @@
       <c r="H156" s="3"/>
       <c r="I156"/>
     </row>
-    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>2</v>
       </c>
@@ -8573,7 +8572,7 @@
       <c r="H164" s="3"/>
       <c r="I164"/>
     </row>
-    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>2</v>
       </c>
@@ -8598,7 +8597,7 @@
       <c r="H165" s="3"/>
       <c r="I165"/>
     </row>
-    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>2</v>
       </c>
@@ -8623,7 +8622,7 @@
       <c r="H166" s="3"/>
       <c r="I166"/>
     </row>
-    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>2</v>
       </c>
@@ -8650,7 +8649,7 @@
       </c>
       <c r="I167"/>
     </row>
-    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>2</v>
       </c>
@@ -9229,7 +9228,7 @@
       <c r="H192" s="3"/>
       <c r="I192"/>
     </row>
-    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>2</v>
       </c>
@@ -9254,7 +9253,7 @@
       <c r="H193" s="3"/>
       <c r="I193"/>
     </row>
-    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>2</v>
       </c>
@@ -9279,7 +9278,7 @@
       <c r="H194" s="3"/>
       <c r="I194"/>
     </row>
-    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>2</v>
       </c>
@@ -9306,7 +9305,7 @@
       </c>
       <c r="I195"/>
     </row>
-    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>2</v>
       </c>
@@ -9563,7 +9562,7 @@
       <c r="H206" s="3"/>
       <c r="I206"/>
     </row>
-    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>2</v>
       </c>
@@ -9590,7 +9589,7 @@
       </c>
       <c r="I207"/>
     </row>
-    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>2</v>
       </c>
@@ -9617,7 +9616,7 @@
       </c>
       <c r="I208"/>
     </row>
-    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>2</v>
       </c>
@@ -9644,7 +9643,7 @@
       </c>
       <c r="I209"/>
     </row>
-    <row r="210" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>2</v>
       </c>
@@ -9671,7 +9670,7 @@
       </c>
       <c r="I210"/>
     </row>
-    <row r="211" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>2</v>
       </c>
@@ -9698,7 +9697,7 @@
       </c>
       <c r="I211"/>
     </row>
-    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>2</v>
       </c>
@@ -9909,7 +9908,7 @@
       <c r="H220" s="3"/>
       <c r="I220"/>
     </row>
-    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>2</v>
       </c>
@@ -9934,7 +9933,7 @@
       <c r="H221" s="3"/>
       <c r="I221"/>
     </row>
-    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>2</v>
       </c>
@@ -9959,7 +9958,7 @@
       <c r="H222" s="3"/>
       <c r="I222"/>
     </row>
-    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>2</v>
       </c>
@@ -9984,7 +9983,7 @@
       <c r="H223" s="3"/>
       <c r="I223"/>
     </row>
-    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>2</v>
       </c>
@@ -10009,7 +10008,7 @@
       <c r="H224" s="3"/>
       <c r="I224"/>
     </row>
-    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>2</v>
       </c>
@@ -10034,7 +10033,7 @@
       <c r="H225" s="3"/>
       <c r="I225"/>
     </row>
-    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>2</v>
       </c>
@@ -10105,7 +10104,7 @@
       <c r="H228" s="3"/>
       <c r="I228"/>
     </row>
-    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>2</v>
       </c>
@@ -10132,7 +10131,7 @@
       </c>
       <c r="I229"/>
     </row>
-    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>2</v>
       </c>
@@ -10374,7 +10373,7 @@
       <c r="H239" s="3"/>
       <c r="I239"/>
     </row>
-    <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>2</v>
       </c>
@@ -10399,7 +10398,7 @@
       <c r="H240" s="3"/>
       <c r="I240"/>
     </row>
-    <row r="241" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>2</v>
       </c>
@@ -10631,7 +10630,7 @@
       <c r="H250" s="3"/>
       <c r="I250"/>
     </row>
-    <row r="251" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>2</v>
       </c>
@@ -10658,7 +10657,7 @@
       </c>
       <c r="I251"/>
     </row>
-    <row r="252" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>2</v>
       </c>
@@ -11007,7 +11006,7 @@
       <c r="H266" s="3"/>
       <c r="I266"/>
     </row>
-    <row r="267" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>2</v>
       </c>
@@ -11034,7 +11033,7 @@
       </c>
       <c r="I267"/>
     </row>
-    <row r="268" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>2</v>
       </c>
@@ -11061,7 +11060,7 @@
       </c>
       <c r="I268"/>
     </row>
-    <row r="269" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>2</v>
       </c>
@@ -11272,7 +11271,7 @@
       <c r="H277" s="3"/>
       <c r="I277"/>
     </row>
-    <row r="278" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>2</v>
       </c>
@@ -11299,7 +11298,7 @@
       </c>
       <c r="I278"/>
     </row>
-    <row r="279" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
         <v>2</v>
       </c>
@@ -11326,7 +11325,7 @@
       </c>
       <c r="I279"/>
     </row>
-    <row r="280" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>2</v>
       </c>
@@ -11353,7 +11352,7 @@
       </c>
       <c r="I280"/>
     </row>
-    <row r="281" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>2</v>
       </c>
@@ -11587,7 +11586,7 @@
       <c r="H290" s="3"/>
       <c r="I290"/>
     </row>
-    <row r="291" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A291" s="1">
         <v>2</v>
       </c>
@@ -11614,7 +11613,7 @@
       </c>
       <c r="I291"/>
     </row>
-    <row r="292" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A292" s="1">
         <v>2</v>
       </c>
@@ -11641,7 +11640,7 @@
       </c>
       <c r="I292"/>
     </row>
-    <row r="293" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
         <v>2</v>
       </c>
@@ -11668,7 +11667,7 @@
       </c>
       <c r="I293"/>
     </row>
-    <row r="294" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A294" s="1">
         <v>2</v>
       </c>
@@ -11904,7 +11903,7 @@
       <c r="H303" s="3"/>
       <c r="I303"/>
     </row>
-    <row r="304" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A304" s="1">
         <v>2</v>
       </c>
@@ -11931,7 +11930,7 @@
       </c>
       <c r="I304"/>
     </row>
-    <row r="305" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A305" s="1">
         <v>2</v>
       </c>
@@ -11958,7 +11957,7 @@
       </c>
       <c r="I305"/>
     </row>
-    <row r="306" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A306" s="1">
         <v>2</v>
       </c>
@@ -11985,7 +11984,7 @@
       </c>
       <c r="I306"/>
     </row>
-    <row r="307" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A307" s="1">
         <v>2</v>
       </c>
@@ -12219,7 +12218,7 @@
       <c r="H316" s="3"/>
       <c r="I316"/>
     </row>
-    <row r="317" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
         <v>2</v>
       </c>
@@ -12346,7 +12345,7 @@
       </c>
       <c r="I321"/>
     </row>
-    <row r="322" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A322" s="9">
         <v>2</v>
       </c>
@@ -12578,7 +12577,7 @@
       <c r="H331" s="3"/>
       <c r="I331"/>
     </row>
-    <row r="332" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A332" s="1">
         <v>2</v>
       </c>
@@ -12605,7 +12604,7 @@
       </c>
       <c r="I332"/>
     </row>
-    <row r="333" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A333" s="1">
         <v>2</v>
       </c>
@@ -12983,7 +12982,7 @@
       <c r="H348" s="3"/>
       <c r="I348"/>
     </row>
-    <row r="349" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A349" s="1">
         <v>2</v>
       </c>
@@ -13010,7 +13009,7 @@
       </c>
       <c r="I349"/>
     </row>
-    <row r="350" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A350" s="1">
         <v>2</v>
       </c>
@@ -13037,7 +13036,7 @@
       </c>
       <c r="I350"/>
     </row>
-    <row r="351" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A351" s="1">
         <v>2</v>
       </c>
@@ -13064,7 +13063,7 @@
       </c>
       <c r="I351"/>
     </row>
-    <row r="352" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A352" s="1">
         <v>2</v>
       </c>
@@ -13091,7 +13090,7 @@
       </c>
       <c r="I352"/>
     </row>
-    <row r="353" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A353" s="1">
         <v>2</v>
       </c>
@@ -13118,7 +13117,7 @@
       </c>
       <c r="I353"/>
     </row>
-    <row r="354" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A354" s="1">
         <v>2</v>
       </c>
@@ -13283,7 +13282,7 @@
       <c r="H360" s="3"/>
       <c r="I360"/>
     </row>
-    <row r="361" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A361" s="1">
         <v>2</v>
       </c>
@@ -13310,7 +13309,7 @@
       </c>
       <c r="I361"/>
     </row>
-    <row r="362" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A362" s="1">
         <v>2</v>
       </c>
@@ -13337,7 +13336,7 @@
       </c>
       <c r="I362"/>
     </row>
-    <row r="363" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A363" s="1">
         <v>2</v>
       </c>
@@ -13364,7 +13363,7 @@
       </c>
       <c r="I363"/>
     </row>
-    <row r="364" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A364" s="1">
         <v>2</v>
       </c>
@@ -13391,7 +13390,7 @@
       </c>
       <c r="I364"/>
     </row>
-    <row r="365" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A365" s="1">
         <v>2</v>
       </c>
@@ -13464,7 +13463,7 @@
       <c r="H367" s="3"/>
       <c r="I367"/>
     </row>
-    <row r="368" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A368" s="1">
         <v>2</v>
       </c>
@@ -13491,7 +13490,7 @@
       </c>
       <c r="I368"/>
     </row>
-    <row r="369" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A369" s="1">
         <v>2</v>
       </c>
@@ -13518,7 +13517,7 @@
       </c>
       <c r="I369"/>
     </row>
-    <row r="370" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A370" s="1">
         <v>2</v>
       </c>
@@ -13687,7 +13686,7 @@
       <c r="H376" s="3"/>
       <c r="I376"/>
     </row>
-    <row r="377" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A377" s="1">
         <v>2</v>
       </c>
@@ -13714,7 +13713,7 @@
       </c>
       <c r="I377"/>
     </row>
-    <row r="378" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A378" s="1">
         <v>2</v>
       </c>
@@ -13833,7 +13832,7 @@
       <c r="H382" s="3"/>
       <c r="I382"/>
     </row>
-    <row r="383" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A383" s="1">
         <v>2</v>
       </c>
@@ -13860,7 +13859,7 @@
       </c>
       <c r="I383"/>
     </row>
-    <row r="384" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A384" s="1">
         <v>2</v>
       </c>
@@ -13887,7 +13886,7 @@
       </c>
       <c r="I384"/>
     </row>
-    <row r="385" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A385" s="1">
         <v>2</v>
       </c>
@@ -13914,7 +13913,7 @@
       </c>
       <c r="I385"/>
     </row>
-    <row r="386" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A386" s="1">
         <v>2</v>
       </c>
@@ -13941,7 +13940,7 @@
       </c>
       <c r="I386"/>
     </row>
-    <row r="387" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A387" s="1">
         <v>2</v>
       </c>
@@ -14359,7 +14358,7 @@
       <c r="H404" s="3"/>
       <c r="I404"/>
     </row>
-    <row r="405" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A405" s="1">
         <v>2</v>
       </c>
@@ -14386,7 +14385,7 @@
       </c>
       <c r="I405"/>
     </row>
-    <row r="406" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A406" s="1">
         <v>2</v>
       </c>
@@ -14413,7 +14412,7 @@
       </c>
       <c r="I406"/>
     </row>
-    <row r="407" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A407" s="1">
         <v>2</v>
       </c>
@@ -14532,7 +14531,7 @@
       <c r="H411" s="3"/>
       <c r="I411"/>
     </row>
-    <row r="412" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A412" s="1">
         <v>2</v>
       </c>
@@ -14559,7 +14558,7 @@
       </c>
       <c r="I412"/>
     </row>
-    <row r="413" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A413" s="1">
         <v>2</v>
       </c>
@@ -14661,7 +14660,7 @@
       </c>
       <c r="I416"/>
     </row>
-    <row r="417" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A417" s="1">
         <v>2</v>
       </c>
@@ -14688,7 +14687,7 @@
       </c>
       <c r="I417"/>
     </row>
-    <row r="418" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A418" s="1">
         <v>2</v>
       </c>
@@ -14715,7 +14714,7 @@
       </c>
       <c r="I418"/>
     </row>
-    <row r="419" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A419" s="1">
         <v>2</v>
       </c>
@@ -14742,7 +14741,7 @@
       </c>
       <c r="I419"/>
     </row>
-    <row r="420" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A420" s="1">
         <v>2</v>
       </c>
@@ -14861,7 +14860,7 @@
       <c r="H424" s="3"/>
       <c r="I424"/>
     </row>
-    <row r="425" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A425" s="1">
         <v>2</v>
       </c>
@@ -14888,7 +14887,7 @@
       </c>
       <c r="I425"/>
     </row>
-    <row r="426" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A426" s="1">
         <v>2</v>
       </c>
@@ -15007,7 +15006,7 @@
       <c r="H430" s="3"/>
       <c r="I430"/>
     </row>
-    <row r="431" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A431" s="1">
         <v>2</v>
       </c>
@@ -15034,7 +15033,7 @@
       </c>
       <c r="I431"/>
     </row>
-    <row r="432" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A432" s="1">
         <v>2</v>
       </c>
@@ -15061,7 +15060,7 @@
       </c>
       <c r="I432"/>
     </row>
-    <row r="433" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A433" s="1">
         <v>2</v>
       </c>
@@ -15203,7 +15202,7 @@
       <c r="H438" s="3"/>
       <c r="I438"/>
     </row>
-    <row r="439" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A439" s="1">
         <v>2</v>
       </c>
@@ -15228,7 +15227,7 @@
       <c r="H439" s="3"/>
       <c r="I439"/>
     </row>
-    <row r="440" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A440" s="1">
         <v>2</v>
       </c>
@@ -15253,7 +15252,7 @@
       <c r="H440" s="3"/>
       <c r="I440"/>
     </row>
-    <row r="441" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A441" s="1">
         <v>2</v>
       </c>
@@ -15278,7 +15277,7 @@
       <c r="H441" s="3"/>
       <c r="I441"/>
     </row>
-    <row r="442" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A442" s="1">
         <v>2</v>
       </c>
@@ -15602,7 +15601,7 @@
       <c r="H455" s="3"/>
       <c r="I455"/>
     </row>
-    <row r="456" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A456" s="1">
         <v>2</v>
       </c>
@@ -15627,7 +15626,7 @@
       <c r="H456" s="3"/>
       <c r="I456"/>
     </row>
-    <row r="457" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A457" s="1">
         <v>2</v>
       </c>
@@ -15652,7 +15651,7 @@
       <c r="H457" s="3"/>
       <c r="I457"/>
     </row>
-    <row r="458" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A458" s="1">
         <v>2</v>
       </c>
@@ -15677,7 +15676,7 @@
       <c r="H458" s="3"/>
       <c r="I458"/>
     </row>
-    <row r="459" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A459" s="1">
         <v>2</v>
       </c>
@@ -15704,7 +15703,7 @@
       </c>
       <c r="I459"/>
     </row>
-    <row r="460" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A460" s="1">
         <v>2</v>
       </c>
@@ -15919,7 +15918,7 @@
       </c>
       <c r="I468"/>
     </row>
-    <row r="469" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A469" s="1">
         <v>2</v>
       </c>
@@ -15946,7 +15945,7 @@
       </c>
       <c r="I469"/>
     </row>
-    <row r="470" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A470" s="1">
         <v>2</v>
       </c>
@@ -16141,7 +16140,7 @@
       <c r="H477" s="3"/>
       <c r="I477"/>
     </row>
-    <row r="478" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A478" s="1">
         <v>2</v>
       </c>
@@ -16168,7 +16167,7 @@
       </c>
       <c r="I478"/>
     </row>
-    <row r="479" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A479" s="1">
         <v>2</v>
       </c>
@@ -16310,7 +16309,7 @@
       <c r="H484" s="3"/>
       <c r="I484"/>
     </row>
-    <row r="485" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A485" s="1">
         <v>2</v>
       </c>
@@ -16337,7 +16336,7 @@
       </c>
       <c r="I485"/>
     </row>
-    <row r="486" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A486" s="1">
         <v>2</v>
       </c>
@@ -16456,7 +16455,7 @@
       <c r="H490" s="3"/>
       <c r="I490"/>
     </row>
-    <row r="491" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A491" s="1">
         <v>2</v>
       </c>
@@ -16483,7 +16482,7 @@
       </c>
       <c r="I491"/>
     </row>
-    <row r="492" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A492" s="1">
         <v>2</v>
       </c>
@@ -16809,7 +16808,7 @@
       <c r="H505" s="3"/>
       <c r="I505"/>
     </row>
-    <row r="506" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A506" s="1">
         <v>2</v>
       </c>
@@ -16836,7 +16835,7 @@
       </c>
       <c r="I506"/>
     </row>
-    <row r="507" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A507" s="1">
         <v>2</v>
       </c>
@@ -17032,7 +17031,7 @@
       </c>
       <c r="I514"/>
     </row>
-    <row r="515" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A515" s="1">
         <v>2</v>
       </c>
@@ -17059,7 +17058,7 @@
       </c>
       <c r="I515"/>
     </row>
-    <row r="516" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A516" s="1">
         <v>2</v>
       </c>
@@ -17201,7 +17200,7 @@
       <c r="H521" s="3"/>
       <c r="I521"/>
     </row>
-    <row r="522" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="522" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A522" s="1">
         <v>2</v>
       </c>
@@ -17228,7 +17227,7 @@
       </c>
       <c r="I522"/>
     </row>
-    <row r="523" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="523" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A523" s="1">
         <v>2</v>
       </c>
@@ -17255,7 +17254,7 @@
       </c>
       <c r="I523"/>
     </row>
-    <row r="524" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="524" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A524" s="1">
         <v>2</v>
       </c>
@@ -17282,7 +17281,7 @@
       </c>
       <c r="I524"/>
     </row>
-    <row r="525" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="525" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A525" s="1">
         <v>2</v>
       </c>
@@ -17447,7 +17446,7 @@
       <c r="H531" s="3"/>
       <c r="I531"/>
     </row>
-    <row r="532" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="532" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A532" s="1">
         <v>2</v>
       </c>
@@ -17474,7 +17473,7 @@
       </c>
       <c r="I532"/>
     </row>
-    <row r="533" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A533" s="1">
         <v>2</v>
       </c>
@@ -17593,7 +17592,7 @@
       <c r="H537" s="3"/>
       <c r="I537"/>
     </row>
-    <row r="538" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="538" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A538" s="1">
         <v>2</v>
       </c>
@@ -17620,7 +17619,7 @@
       </c>
       <c r="I538"/>
     </row>
-    <row r="539" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="539" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A539" s="1">
         <v>2</v>
       </c>
@@ -17879,7 +17878,7 @@
       <c r="H549" s="3"/>
       <c r="I549"/>
     </row>
-    <row r="550" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="550" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A550" s="1">
         <v>2</v>
       </c>
@@ -17906,7 +17905,7 @@
       </c>
       <c r="I550"/>
     </row>
-    <row r="551" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="551" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A551" s="1">
         <v>2</v>
       </c>
@@ -17933,7 +17932,7 @@
       </c>
       <c r="I551"/>
     </row>
-    <row r="552" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="552" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A552" s="1">
         <v>2</v>
       </c>
@@ -17960,7 +17959,7 @@
       </c>
       <c r="I552"/>
     </row>
-    <row r="553" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="553" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A553" s="1">
         <v>2</v>
       </c>
@@ -17987,7 +17986,7 @@
       </c>
       <c r="I553"/>
     </row>
-    <row r="554" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="554" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A554" s="1">
         <v>2</v>
       </c>
@@ -18135,7 +18134,7 @@
       <c r="H559" s="3"/>
       <c r="I559"/>
     </row>
-    <row r="560" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="560" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A560" s="1">
         <v>2</v>
       </c>
@@ -18162,7 +18161,7 @@
       </c>
       <c r="I560"/>
     </row>
-    <row r="561" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A561" s="1">
         <v>2</v>
       </c>
@@ -18421,7 +18420,7 @@
       <c r="H571" s="3"/>
       <c r="I571"/>
     </row>
-    <row r="572" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="572" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A572" s="1">
         <v>2</v>
       </c>
@@ -18448,7 +18447,7 @@
       </c>
       <c r="I572"/>
     </row>
-    <row r="573" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="573" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A573" s="1">
         <v>2</v>
       </c>
@@ -18567,7 +18566,7 @@
       <c r="H577" s="3"/>
       <c r="I577"/>
     </row>
-    <row r="578" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="578" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A578" s="1">
         <v>2</v>
       </c>
@@ -18594,7 +18593,7 @@
       </c>
       <c r="I578"/>
     </row>
-    <row r="579" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="579" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A579" s="1">
         <v>2</v>
       </c>
@@ -18782,7 +18781,7 @@
       <c r="H586" s="3"/>
       <c r="I586"/>
     </row>
-    <row r="587" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="587" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A587" s="1">
         <v>3</v>
       </c>
@@ -18809,7 +18808,7 @@
       </c>
       <c r="I587"/>
     </row>
-    <row r="588" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="588" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A588" s="1">
         <v>3</v>
       </c>
@@ -18836,7 +18835,7 @@
       </c>
       <c r="I588"/>
     </row>
-    <row r="589" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="589" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A589" s="1">
         <v>3</v>
       </c>
@@ -18863,7 +18862,7 @@
       </c>
       <c r="I589"/>
     </row>
-    <row r="590" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="590" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A590" s="1">
         <v>3</v>
       </c>
@@ -19571,7 +19570,7 @@
       <c r="H619" s="3"/>
       <c r="I619"/>
     </row>
-    <row r="620" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="620" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A620" s="9">
         <v>3</v>
       </c>
@@ -19596,7 +19595,7 @@
       </c>
       <c r="I620"/>
     </row>
-    <row r="621" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="621" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A621" s="1">
         <v>3</v>
       </c>
@@ -19784,7 +19783,7 @@
       <c r="H628" s="3"/>
       <c r="I628"/>
     </row>
-    <row r="629" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="629" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A629" s="1">
         <v>3</v>
       </c>
@@ -19809,7 +19808,7 @@
       <c r="H629" s="3"/>
       <c r="I629"/>
     </row>
-    <row r="630" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="630" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A630" s="1">
         <v>3</v>
       </c>
@@ -19834,7 +19833,7 @@
       <c r="H630" s="3"/>
       <c r="I630"/>
     </row>
-    <row r="631" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="631" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A631" s="1">
         <v>3</v>
       </c>
@@ -19997,7 +19996,7 @@
       <c r="H637" s="3"/>
       <c r="I637"/>
     </row>
-    <row r="638" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="638" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A638" s="1">
         <v>3</v>
       </c>
@@ -20022,7 +20021,7 @@
       <c r="H638" s="3"/>
       <c r="I638"/>
     </row>
-    <row r="639" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="639" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A639" s="1">
         <v>3</v>
       </c>
@@ -20047,7 +20046,7 @@
       <c r="H639" s="3"/>
       <c r="I639"/>
     </row>
-    <row r="640" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="640" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A640" s="1">
         <v>3</v>
       </c>
@@ -20348,7 +20347,7 @@
       <c r="H652" s="3"/>
       <c r="I652"/>
     </row>
-    <row r="653" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="653" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A653" s="1">
         <v>3</v>
       </c>
@@ -20373,7 +20372,7 @@
       <c r="H653" s="3"/>
       <c r="I653"/>
     </row>
-    <row r="654" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="654" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A654" s="1">
         <v>3</v>
       </c>
@@ -20881,7 +20880,7 @@
       <c r="H675" s="3"/>
       <c r="I675"/>
     </row>
-    <row r="676" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="676" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A676" s="1">
         <v>3</v>
       </c>
@@ -20908,7 +20907,7 @@
       </c>
       <c r="I676"/>
     </row>
-    <row r="677" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="677" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A677" s="1">
         <v>3</v>
       </c>
@@ -20935,7 +20934,7 @@
       </c>
       <c r="I677"/>
     </row>
-    <row r="678" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="678" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A678" s="1">
         <v>3</v>
       </c>
@@ -20962,7 +20961,7 @@
       </c>
       <c r="I678"/>
     </row>
-    <row r="679" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="679" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A679" s="1">
         <v>3</v>
       </c>
@@ -23065,7 +23064,7 @@
       <c r="H769" s="3"/>
       <c r="I769"/>
     </row>
-    <row r="770" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="770" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A770" s="1">
         <v>4</v>
       </c>
@@ -23090,7 +23089,7 @@
       <c r="H770" s="3"/>
       <c r="I770"/>
     </row>
-    <row r="771" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="771" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A771" s="1">
         <v>4</v>
       </c>
@@ -23115,7 +23114,7 @@
       <c r="H771" s="3"/>
       <c r="I771"/>
     </row>
-    <row r="772" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="772" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A772" s="1">
         <v>4</v>
       </c>
@@ -23209,7 +23208,7 @@
       <c r="H775" s="3"/>
       <c r="I775"/>
     </row>
-    <row r="776" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="776" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A776" s="1">
         <v>4</v>
       </c>
@@ -23236,7 +23235,7 @@
       </c>
       <c r="I776"/>
     </row>
-    <row r="777" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="777" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A777" s="1">
         <v>4</v>
       </c>
@@ -23378,7 +23377,7 @@
       <c r="H782" s="3"/>
       <c r="I782"/>
     </row>
-    <row r="783" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="783" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A783" s="1">
         <v>4</v>
       </c>
@@ -23405,7 +23404,7 @@
       </c>
       <c r="I783"/>
     </row>
-    <row r="784" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="784" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A784" s="1">
         <v>4</v>
       </c>
@@ -23576,7 +23575,7 @@
       <c r="H790" s="3"/>
       <c r="I790"/>
     </row>
-    <row r="791" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="791" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A791" s="1">
         <v>4</v>
       </c>
@@ -23601,7 +23600,7 @@
       <c r="H791" s="3"/>
       <c r="I791"/>
     </row>
-    <row r="792" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="792" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A792" s="1">
         <v>4</v>
       </c>
@@ -23626,7 +23625,7 @@
       <c r="H792" s="3"/>
       <c r="I792"/>
     </row>
-    <row r="793" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="793" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A793" s="1">
         <v>4</v>
       </c>
@@ -23651,7 +23650,7 @@
       <c r="H793" s="3"/>
       <c r="I793"/>
     </row>
-    <row r="794" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="794" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A794" s="1">
         <v>4</v>
       </c>
@@ -23676,7 +23675,7 @@
       <c r="H794" s="3"/>
       <c r="I794"/>
     </row>
-    <row r="795" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="795" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A795" s="1">
         <v>4</v>
       </c>
@@ -23701,7 +23700,7 @@
       <c r="H795" s="3"/>
       <c r="I795"/>
     </row>
-    <row r="796" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="796" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A796" s="2">
         <v>4</v>
       </c>

</xml_diff>